<commit_message>
add support for seeding
</commit_message>
<xml_diff>
--- a/agave/help/BracketDefsSample.xlsx
+++ b/agave/help/BracketDefsSample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26926"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\bbld\agave\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\bbld\agave\help\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45CAFF4C-31C8-4563-A306-69D9EEE0EC01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5027295C-B3A4-45E3-8376-66F6EEEBFD31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12920" yWindow="1460" windowWidth="22550" windowHeight="18530" xr2:uid="{52C424EE-47AA-4076-837E-9FEA6E181BB1}"/>
+    <workbookView xWindow="39990" yWindow="2650" windowWidth="24410" windowHeight="16440" xr2:uid="{52C424EE-47AA-4076-837E-9FEA6E181BB1}"/>
   </bookViews>
   <sheets>
     <sheet name="BracketDefs" sheetId="2" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="205">
   <si>
     <t>2 Team</t>
   </si>
@@ -613,6 +613,54 @@
   </si>
   <si>
     <t>W38</t>
+  </si>
+  <si>
+    <t>TopSeedName</t>
+  </si>
+  <si>
+    <t>BottomSeedName</t>
+  </si>
+  <si>
+    <t>Seed 1</t>
+  </si>
+  <si>
+    <t>Seed 2</t>
+  </si>
+  <si>
+    <t>Seed 3</t>
+  </si>
+  <si>
+    <t>Seed 4</t>
+  </si>
+  <si>
+    <t>Seed 5</t>
+  </si>
+  <si>
+    <t>Seed 6</t>
+  </si>
+  <si>
+    <t>Seed 7</t>
+  </si>
+  <si>
+    <t>Seed 10</t>
+  </si>
+  <si>
+    <t>Seed 11</t>
+  </si>
+  <si>
+    <t>Seed 8</t>
+  </si>
+  <si>
+    <t>Seed 9</t>
+  </si>
+  <si>
+    <t>Seed 12</t>
+  </si>
+  <si>
+    <t>Seed 13</t>
+  </si>
+  <si>
+    <t>Seed 14</t>
   </si>
 </sst>
 </file>
@@ -705,9 +753,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F79377BF-F9E2-4624-A542-5222D8F2DC5B}" name="T2Bracket" displayName="T2Bracket" ref="B4:H8" totalsRowShown="0">
-  <autoFilter ref="B4:H8" xr:uid="{F79377BF-F9E2-4624-A542-5222D8F2DC5B}"/>
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F79377BF-F9E2-4624-A542-5222D8F2DC5B}" name="T2Bracket" displayName="T2Bracket" ref="B4:J8" totalsRowShown="0">
+  <autoFilter ref="B4:J8" xr:uid="{F79377BF-F9E2-4624-A542-5222D8F2DC5B}"/>
+  <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{CA12300B-71E2-48E0-A0F9-FE229F3C5098}" name="Game"/>
     <tableColumn id="2" xr3:uid="{398BBF8E-29FB-4001-BA58-61F7160B7DF0}" name="Winner"/>
     <tableColumn id="3" xr3:uid="{FF46934E-5C58-4DFA-8B38-A85260AB5C2E}" name="Loser"/>
@@ -719,15 +767,17 @@
     <tableColumn id="7" xr3:uid="{8D170CF2-EF0F-4272-800C-AD15D613F846}" name="CountBottomCheck" dataDxfId="10">
       <calculatedColumnFormula>COUNTIF(T2Bracket[[Winner]:[Loser]], "B" &amp; T2Bracket[[#This Row],[Game]])</calculatedColumnFormula>
     </tableColumn>
+    <tableColumn id="8" xr3:uid="{0CBFC66D-E466-47D0-AE20-3DD2ED738A54}" name="TopSeedName"/>
+    <tableColumn id="9" xr3:uid="{A6A6007E-9C21-4E97-B7ED-8C457C48418D}" name="BottomSeedName"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{AD5777E6-3D08-427F-BAAB-E98368E6298D}" name="T3Bracket" displayName="T3Bracket" ref="B17:H23" totalsRowShown="0">
-  <autoFilter ref="B17:H23" xr:uid="{AD5777E6-3D08-427F-BAAB-E98368E6298D}"/>
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{AD5777E6-3D08-427F-BAAB-E98368E6298D}" name="T3Bracket" displayName="T3Bracket" ref="B17:J23" totalsRowShown="0">
+  <autoFilter ref="B17:J23" xr:uid="{AD5777E6-3D08-427F-BAAB-E98368E6298D}"/>
+  <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{E246C55C-41D7-4163-A14B-124B3B4D01A4}" name="Game"/>
     <tableColumn id="2" xr3:uid="{520E1BC6-0753-428C-8FD2-3DD88134AA8A}" name="Winner"/>
     <tableColumn id="3" xr3:uid="{B5DEAED6-784F-4FCC-B544-792841636E51}" name="Loser"/>
@@ -739,15 +789,17 @@
     <tableColumn id="7" xr3:uid="{5032FB3F-FAC6-41C6-830D-21A859C255F7}" name="CountBottomCheck" dataDxfId="8">
       <calculatedColumnFormula>COUNTIF(T3Bracket[[Winner]:[Loser]], "B" &amp; T3Bracket[[#This Row],[Game]])</calculatedColumnFormula>
     </tableColumn>
+    <tableColumn id="8" xr3:uid="{2D363F72-ECD5-44FC-9B4A-1DF19E2E39A8}" name="TopSeedName"/>
+    <tableColumn id="9" xr3:uid="{9FA296DF-CAC0-4266-9895-B861CA5A25A1}" name="BottomSeedName"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{AEC439CE-9C1A-48E7-8C83-AFE0A245B968}" name="T4Bracket" displayName="T4Bracket" ref="B32:H39" totalsRowShown="0">
-  <autoFilter ref="B32:H39" xr:uid="{AEC439CE-9C1A-48E7-8C83-AFE0A245B968}"/>
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{AEC439CE-9C1A-48E7-8C83-AFE0A245B968}" name="T4Bracket" displayName="T4Bracket" ref="B32:J39" totalsRowShown="0">
+  <autoFilter ref="B32:J39" xr:uid="{AEC439CE-9C1A-48E7-8C83-AFE0A245B968}"/>
+  <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{13756E6D-4979-4845-932E-FD54EE234BE1}" name="Game"/>
     <tableColumn id="2" xr3:uid="{B231DC6D-81CE-4549-A90E-9BFF2AC77313}" name="Winner"/>
     <tableColumn id="3" xr3:uid="{41A8C26F-4C1F-4D11-B521-D8D50CC74F1B}" name="Loser"/>
@@ -759,15 +811,17 @@
     <tableColumn id="7" xr3:uid="{E1222CD2-BE33-4699-9863-E41B6F0E0ACA}" name="CountBottomCheck" dataDxfId="6">
       <calculatedColumnFormula>COUNTIF(T4Bracket[[Winner]:[Loser]], "B" &amp; T4Bracket[[#This Row],[Game]])</calculatedColumnFormula>
     </tableColumn>
+    <tableColumn id="8" xr3:uid="{C37F225B-ADCB-46AA-BBF9-3AA9FC8CEC71}" name="TopSeedName"/>
+    <tableColumn id="9" xr3:uid="{D5F0A381-4E3F-4374-A163-115E5F8E660F}" name="BottomSeedName"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{768D792C-2ACA-46AD-9F73-FC8714D5B713}" name="T5Bracket" displayName="T5Bracket" ref="B48:H58" totalsRowShown="0">
-  <autoFilter ref="B48:H58" xr:uid="{768D792C-2ACA-46AD-9F73-FC8714D5B713}"/>
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{768D792C-2ACA-46AD-9F73-FC8714D5B713}" name="T5Bracket" displayName="T5Bracket" ref="B48:J58" totalsRowShown="0">
+  <autoFilter ref="B48:J58" xr:uid="{768D792C-2ACA-46AD-9F73-FC8714D5B713}"/>
+  <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{5CB6F2B2-F0ED-4B04-BFEE-F0C60E8F02A3}" name="Game"/>
     <tableColumn id="2" xr3:uid="{BAA2F22C-7859-4A0E-B9B9-3BBDABFFD350}" name="Winner"/>
     <tableColumn id="3" xr3:uid="{6E95D113-F927-491A-98A6-000BE5FAB6CF}" name="Loser"/>
@@ -779,15 +833,17 @@
     <tableColumn id="7" xr3:uid="{4B091951-8AD0-447C-B74F-044A7F847939}" name="CountBottomCheck" dataDxfId="4">
       <calculatedColumnFormula>COUNTIF(T5Bracket[[Winner]:[Loser]], "B" &amp; T5Bracket[[#This Row],[Game]])</calculatedColumnFormula>
     </tableColumn>
+    <tableColumn id="8" xr3:uid="{A5429222-1267-4512-92DB-C35CD0C4A4C2}" name="TopSeedName"/>
+    <tableColumn id="9" xr3:uid="{400CF279-351F-4423-B595-92DAC571BAC6}" name="BottomSeedName"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{1246DDCF-9449-4A94-AF31-694D53BCB8F3}" name="T6Bracket" displayName="T6Bracket" ref="B67:H79" totalsRowShown="0">
-  <autoFilter ref="B67:H79" xr:uid="{1246DDCF-9449-4A94-AF31-694D53BCB8F3}"/>
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{1246DDCF-9449-4A94-AF31-694D53BCB8F3}" name="T6Bracket" displayName="T6Bracket" ref="B67:J79" totalsRowShown="0">
+  <autoFilter ref="B67:J79" xr:uid="{1246DDCF-9449-4A94-AF31-694D53BCB8F3}"/>
+  <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{10468AD0-0028-409D-A519-E7403825CF4A}" name="Game"/>
     <tableColumn id="2" xr3:uid="{2E5FA294-D136-4004-AC2E-5DDC4F667191}" name="Winner"/>
     <tableColumn id="3" xr3:uid="{C0899572-B8F1-4A3C-A6B8-36B341BEDE97}" name="Loser"/>
@@ -799,15 +855,17 @@
     <tableColumn id="7" xr3:uid="{B2576887-716C-47E4-B0EA-204BF4C2FC2A}" name="CountBottomCheck" dataDxfId="2">
       <calculatedColumnFormula>COUNTIF(T6Bracket[[Winner]:[Loser]], "B" &amp; T6Bracket[[#This Row],[Game]])</calculatedColumnFormula>
     </tableColumn>
+    <tableColumn id="8" xr3:uid="{95F45FC6-BDD6-4505-8A32-7559D2D57D82}" name="TopSeedName"/>
+    <tableColumn id="9" xr3:uid="{4BEFF380-AD0D-4470-911E-6DD03AF7A2C2}" name="BottomSeedName"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{0E3BCB4E-7794-4AD0-9B38-1CA01354EE30}" name="T14Bracket" displayName="T14Bracket" ref="B88:H116" totalsRowShown="0">
-  <autoFilter ref="B88:H116" xr:uid="{0E3BCB4E-7794-4AD0-9B38-1CA01354EE30}"/>
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{0E3BCB4E-7794-4AD0-9B38-1CA01354EE30}" name="T14Bracket" displayName="T14Bracket" ref="B88:J116" totalsRowShown="0">
+  <autoFilter ref="B88:J116" xr:uid="{0E3BCB4E-7794-4AD0-9B38-1CA01354EE30}"/>
+  <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{38B52B4E-5942-4AC3-ABBA-CD948C262CC8}" name="Game"/>
     <tableColumn id="2" xr3:uid="{BE3F375D-2AA1-4520-AEAF-C97E955D92BE}" name="Winner"/>
     <tableColumn id="3" xr3:uid="{FF313F9C-85A6-41CA-86A7-9AFEC432DBFD}" name="Loser"/>
@@ -819,6 +877,8 @@
     <tableColumn id="7" xr3:uid="{275424D1-C3F8-4E5E-A9D6-6190581DEC5A}" name="CountBottomCheck" dataDxfId="0">
       <calculatedColumnFormula>COUNTIF(T14Bracket[[Winner]:[Loser]], "B" &amp; T14Bracket[[#This Row],[Game]])</calculatedColumnFormula>
     </tableColumn>
+    <tableColumn id="8" xr3:uid="{7F693432-7C5E-4051-A6F3-AE26BF1DE3C6}" name="TopSeedName"/>
+    <tableColumn id="9" xr3:uid="{65D89D61-E477-486E-9C95-27EEAFBA9F53}" name="BottomSeedName"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1161,7 +1221,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="1" width="525" row="6">
+  <wetp:taskpane dockstate="right" visibility="0" width="525" row="6">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
 </wetp:taskpanes>
@@ -1179,24 +1239,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BCF2840-C92F-4022-A3EF-8054574591D3}">
-  <dimension ref="A3:H170"/>
+  <dimension ref="A3:J170"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
-      <selection activeCell="C134" sqref="C134"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="18.81640625" customWidth="1"/>
     <col min="2" max="8" width="10.453125" customWidth="1"/>
+    <col min="9" max="10" width="15.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>1</v>
       </c>
@@ -1218,8 +1279,14 @@
       <c r="H4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I4" t="s">
+        <v>189</v>
+      </c>
+      <c r="J4" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B5">
         <v>1</v>
       </c>
@@ -1243,8 +1310,14 @@
         <f>COUNTIF(T2Bracket[[Winner]:[Loser]], "B" &amp; T2Bracket[[#This Row],[Game]])</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I5" t="s">
+        <v>191</v>
+      </c>
+      <c r="J5" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B6">
         <v>2</v>
       </c>
@@ -1269,7 +1342,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B7">
         <v>3</v>
       </c>
@@ -1291,7 +1364,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B8">
         <v>4</v>
       </c>
@@ -1307,7 +1380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -1316,7 +1389,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -1329,7 +1402,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -1342,7 +1415,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -1355,12 +1428,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
         <v>1</v>
       </c>
@@ -1382,8 +1455,14 @@
       <c r="H17" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I17" t="s">
+        <v>189</v>
+      </c>
+      <c r="J17" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B18">
         <v>1</v>
       </c>
@@ -1407,8 +1486,14 @@
         <f>COUNTIF(T3Bracket[[Winner]:[Loser]], "B" &amp; T3Bracket[[#This Row],[Game]])</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I18" t="s">
+        <v>192</v>
+      </c>
+      <c r="J18" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B19">
         <v>2</v>
       </c>
@@ -1432,8 +1517,11 @@
         <f>COUNTIF(T3Bracket[[Winner]:[Loser]], "B" &amp; T3Bracket[[#This Row],[Game]])</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="J19" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B20">
         <v>3</v>
       </c>
@@ -1455,7 +1543,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B21">
         <v>4</v>
       </c>
@@ -1480,7 +1568,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B22">
         <v>5</v>
       </c>
@@ -1502,7 +1590,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B23">
         <v>6</v>
       </c>
@@ -1518,7 +1606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>20</v>
       </c>
@@ -1527,7 +1615,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>21</v>
       </c>
@@ -1540,7 +1628,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>22</v>
       </c>
@@ -1553,7 +1641,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>23</v>
       </c>
@@ -1566,12 +1654,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B31" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B32" t="s">
         <v>1</v>
       </c>
@@ -1593,8 +1681,14 @@
       <c r="H32" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I32" t="s">
+        <v>189</v>
+      </c>
+      <c r="J32" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B33">
         <v>1</v>
       </c>
@@ -1618,8 +1712,14 @@
         <f>COUNTIF(T4Bracket[[Winner]:[Loser]], "B" &amp; T4Bracket[[#This Row],[Game]])</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I33" t="s">
+        <v>191</v>
+      </c>
+      <c r="J33" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B34">
         <v>2</v>
       </c>
@@ -1643,8 +1743,14 @@
         <f>COUNTIF(T4Bracket[[Winner]:[Loser]], "B" &amp; T4Bracket[[#This Row],[Game]])</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I34" t="s">
+        <v>192</v>
+      </c>
+      <c r="J34" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B35">
         <v>3</v>
       </c>
@@ -1669,7 +1775,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B36">
         <v>4</v>
       </c>
@@ -1691,7 +1797,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B37">
         <v>5</v>
       </c>
@@ -1713,7 +1819,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B38">
         <v>6</v>
       </c>
@@ -1735,7 +1841,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B39">
         <v>7</v>
       </c>
@@ -1751,7 +1857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>20</v>
       </c>
@@ -1760,7 +1866,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>21</v>
       </c>
@@ -1773,7 +1879,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>22</v>
       </c>
@@ -1786,7 +1892,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>23</v>
       </c>
@@ -1799,12 +1905,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B47" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B48" t="s">
         <v>1</v>
       </c>
@@ -1826,8 +1932,14 @@
       <c r="H48" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I48" t="s">
+        <v>189</v>
+      </c>
+      <c r="J48" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B49">
         <v>1</v>
       </c>
@@ -1851,8 +1963,14 @@
         <f>COUNTIF(T5Bracket[[Winner]:[Loser]], "B" &amp; T5Bracket[[#This Row],[Game]])</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I49" t="s">
+        <v>194</v>
+      </c>
+      <c r="J49" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B50">
         <v>2</v>
       </c>
@@ -1876,8 +1994,14 @@
         <f>COUNTIF(T5Bracket[[Winner]:[Loser]], "B" &amp; T5Bracket[[#This Row],[Game]])</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I50" t="s">
+        <v>192</v>
+      </c>
+      <c r="J50" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B51">
         <v>3</v>
       </c>
@@ -1901,8 +2025,11 @@
         <f>COUNTIF(T5Bracket[[Winner]:[Loser]], "B" &amp; T5Bracket[[#This Row],[Game]])</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="J51" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B52">
         <v>4</v>
       </c>
@@ -1924,7 +2051,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B53">
         <v>5</v>
       </c>
@@ -1949,7 +2076,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B54">
         <v>6</v>
       </c>
@@ -1971,7 +2098,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B55">
         <v>7</v>
       </c>
@@ -1993,7 +2120,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B56">
         <v>8</v>
       </c>
@@ -2018,7 +2145,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B57">
         <v>9</v>
       </c>
@@ -2040,7 +2167,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B58">
         <v>10</v>
       </c>
@@ -2056,7 +2183,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>20</v>
       </c>
@@ -2065,7 +2192,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>21</v>
       </c>
@@ -2078,7 +2205,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>22</v>
       </c>
@@ -2091,7 +2218,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>23</v>
       </c>
@@ -2104,12 +2231,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="66" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B66" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="67" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="67" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B67" t="s">
         <v>1</v>
       </c>
@@ -2131,8 +2258,14 @@
       <c r="H67" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="68" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="I67" t="s">
+        <v>189</v>
+      </c>
+      <c r="J67" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="68" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B68">
         <v>1</v>
       </c>
@@ -2156,8 +2289,14 @@
         <f>COUNTIF(T6Bracket[[Winner]:[Loser]], "B" &amp; T6Bracket[[#This Row],[Game]])</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="69" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="I68" t="s">
+        <v>194</v>
+      </c>
+      <c r="J68" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="69" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B69">
         <v>2</v>
       </c>
@@ -2181,8 +2320,14 @@
         <f>COUNTIF(T6Bracket[[Winner]:[Loser]], "B" &amp; T6Bracket[[#This Row],[Game]])</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="70" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="I69" t="s">
+        <v>193</v>
+      </c>
+      <c r="J69" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="70" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B70">
         <v>3</v>
       </c>
@@ -2206,8 +2351,11 @@
         <f>COUNTIF(T6Bracket[[Winner]:[Loser]], "B" &amp; T6Bracket[[#This Row],[Game]])</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="71" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="I70" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="71" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B71">
         <v>4</v>
       </c>
@@ -2231,8 +2379,11 @@
         <f>COUNTIF(T6Bracket[[Winner]:[Loser]], "B" &amp; T6Bracket[[#This Row],[Game]])</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="72" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="J71" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="72" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B72">
         <v>5</v>
       </c>
@@ -2254,7 +2405,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="73" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B73">
         <v>6</v>
       </c>
@@ -2276,7 +2427,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="74" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B74">
         <v>7</v>
       </c>
@@ -2301,7 +2452,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="75" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B75">
         <v>8</v>
       </c>
@@ -2323,7 +2474,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="76" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B76">
         <v>9</v>
       </c>
@@ -2345,7 +2496,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="77" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B77">
         <v>10</v>
       </c>
@@ -2370,7 +2521,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="78" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B78">
         <v>11</v>
       </c>
@@ -2392,7 +2543,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="79" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B79">
         <v>12</v>
       </c>
@@ -2408,7 +2559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>20</v>
       </c>
@@ -2417,7 +2568,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>21</v>
       </c>
@@ -2430,7 +2581,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>22</v>
       </c>
@@ -2443,7 +2594,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>23</v>
       </c>
@@ -2456,12 +2607,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B87" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B88" t="s">
         <v>1</v>
       </c>
@@ -2483,8 +2634,14 @@
       <c r="H88" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I88" t="s">
+        <v>189</v>
+      </c>
+      <c r="J88" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B89">
         <v>1</v>
       </c>
@@ -2508,8 +2665,14 @@
         <f>COUNTIF(T14Bracket[[Winner]:[Loser]], "B" &amp; T14Bracket[[#This Row],[Game]])</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I89" t="s">
+        <v>200</v>
+      </c>
+      <c r="J89" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B90">
         <v>2</v>
       </c>
@@ -2533,8 +2696,14 @@
         <f>COUNTIF(T14Bracket[[Winner]:[Loser]], "B" &amp; T14Bracket[[#This Row],[Game]])</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I90" t="s">
+        <v>195</v>
+      </c>
+      <c r="J90" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B91">
         <v>3</v>
       </c>
@@ -2558,8 +2727,14 @@
         <f>COUNTIF(T14Bracket[[Winner]:[Loser]], "B" &amp; T14Bracket[[#This Row],[Game]])</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I91" t="s">
+        <v>194</v>
+      </c>
+      <c r="J91" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B92">
         <v>4</v>
       </c>
@@ -2583,8 +2758,14 @@
         <f>COUNTIF(T14Bracket[[Winner]:[Loser]], "B" &amp; T14Bracket[[#This Row],[Game]])</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I92" t="s">
+        <v>193</v>
+      </c>
+      <c r="J92" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B93">
         <v>5</v>
       </c>
@@ -2608,8 +2789,14 @@
         <f>COUNTIF(T14Bracket[[Winner]:[Loser]], "B" &amp; T14Bracket[[#This Row],[Game]])</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I93" t="s">
+        <v>196</v>
+      </c>
+      <c r="J93" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B94">
         <v>6</v>
       </c>
@@ -2633,8 +2820,14 @@
         <f>COUNTIF(T14Bracket[[Winner]:[Loser]], "B" &amp; T14Bracket[[#This Row],[Game]])</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I94" t="s">
+        <v>197</v>
+      </c>
+      <c r="J94" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B95">
         <v>7</v>
       </c>
@@ -2658,8 +2851,11 @@
         <f>COUNTIF(T14Bracket[[Winner]:[Loser]], "B" &amp; T14Bracket[[#This Row],[Game]])</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I95" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B96">
         <v>8</v>
       </c>
@@ -2684,7 +2880,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="97" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B97">
         <v>9</v>
       </c>
@@ -2709,7 +2905,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="98" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B98">
         <v>10</v>
       </c>
@@ -2733,8 +2929,11 @@
         <f>COUNTIF(T14Bracket[[Winner]:[Loser]], "B" &amp; T14Bracket[[#This Row],[Game]])</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="99" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="J98" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="99" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B99">
         <v>11</v>
       </c>
@@ -2756,7 +2955,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="100" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B100">
         <v>12</v>
       </c>
@@ -2778,7 +2977,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="101" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B101">
         <v>13</v>
       </c>
@@ -2800,7 +2999,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="102" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B102">
         <v>14</v>
       </c>
@@ -2822,7 +3021,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="103" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B103">
         <v>15</v>
       </c>
@@ -2844,7 +3043,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="104" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B104">
         <v>16</v>
       </c>
@@ -2866,7 +3065,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="105" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B105">
         <v>17</v>
       </c>
@@ -2891,7 +3090,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="106" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B106">
         <v>18</v>
       </c>
@@ -2916,7 +3115,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="107" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B107">
         <v>19</v>
       </c>
@@ -2938,7 +3137,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="108" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B108">
         <v>20</v>
       </c>
@@ -2960,7 +3159,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="109" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B109">
         <v>21</v>
       </c>
@@ -2985,7 +3184,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="110" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B110">
         <v>22</v>
       </c>
@@ -3007,7 +3206,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="111" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B111">
         <v>23</v>
       </c>
@@ -3029,7 +3228,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="112" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B112">
         <v>24</v>
       </c>

</xml_diff>